<commit_message>
agregando version del atu listado
</commit_message>
<xml_diff>
--- a/clean_databases/sp_index.xlsx
+++ b/clean_databases/sp_index.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27510"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargaspoulsen/github/main-fisheries-chile/clean_databases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignacia Rivera\Desktop\GitHub\main-fisheries-chile\clean_databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20779364-35ED-4F2B-8B92-706DD416CC16}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25460" windowHeight="15460"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25455" windowHeight="15465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,24 +20,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="692">
   <si>
     <t>HAEMATOCOCCUS</t>
   </si>
@@ -2109,16 +2104,25 @@
   </si>
   <si>
     <t>VIDRIOLA, PALOMETA, DORADO O TOREMO</t>
+  </si>
+  <si>
+    <t>ATUN LISTADO,BARRILETE,CACHURRETA/AUHOPU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2144,8 +2148,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2459,21 +2464,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C257"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="D159" sqref="D159"/>
+    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
+      <selection activeCell="D254" sqref="D254"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -2484,7 +2489,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -2495,7 +2500,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -2506,7 +2511,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -2517,7 +2522,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -2528,7 +2533,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>83</v>
       </c>
@@ -2539,7 +2544,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>86</v>
       </c>
@@ -2550,7 +2555,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>89</v>
       </c>
@@ -2561,7 +2566,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>92</v>
       </c>
@@ -2572,7 +2577,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -2583,7 +2588,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>98</v>
       </c>
@@ -2594,7 +2599,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -2605,7 +2610,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>104</v>
       </c>
@@ -2616,7 +2621,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>107</v>
       </c>
@@ -2627,7 +2632,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>110</v>
       </c>
@@ -2638,7 +2643,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>111</v>
       </c>
@@ -2649,7 +2654,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>114</v>
       </c>
@@ -2660,7 +2665,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>117</v>
       </c>
@@ -2671,7 +2676,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>119</v>
       </c>
@@ -2682,7 +2687,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>122</v>
       </c>
@@ -2693,7 +2698,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>125</v>
       </c>
@@ -2704,7 +2709,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -2715,7 +2720,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>129</v>
       </c>
@@ -2726,7 +2731,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>130</v>
       </c>
@@ -2737,7 +2742,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>131</v>
       </c>
@@ -2748,7 +2753,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>132</v>
       </c>
@@ -2759,7 +2764,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>135</v>
       </c>
@@ -2770,7 +2775,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>138</v>
       </c>
@@ -2781,7 +2786,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -2792,7 +2797,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>144</v>
       </c>
@@ -2803,7 +2808,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>145</v>
       </c>
@@ -2814,7 +2819,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>148</v>
       </c>
@@ -2825,7 +2830,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>151</v>
       </c>
@@ -2836,7 +2841,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>154</v>
       </c>
@@ -2847,7 +2852,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>685</v>
       </c>
@@ -2858,7 +2863,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>156</v>
       </c>
@@ -2869,7 +2874,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>159</v>
       </c>
@@ -2880,7 +2885,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>162</v>
       </c>
@@ -2891,7 +2896,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>165</v>
       </c>
@@ -2902,7 +2907,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>168</v>
       </c>
@@ -2913,7 +2918,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>171</v>
       </c>
@@ -2924,7 +2929,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>174</v>
       </c>
@@ -2935,7 +2940,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>177</v>
       </c>
@@ -2946,7 +2951,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>180</v>
       </c>
@@ -2957,7 +2962,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>183</v>
       </c>
@@ -2968,7 +2973,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>186</v>
       </c>
@@ -2979,7 +2984,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>189</v>
       </c>
@@ -2990,7 +2995,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>192</v>
       </c>
@@ -3001,7 +3006,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>195</v>
       </c>
@@ -3012,7 +3017,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>198</v>
       </c>
@@ -3023,7 +3028,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>201</v>
       </c>
@@ -3034,7 +3039,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>204</v>
       </c>
@@ -3045,7 +3050,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>207</v>
       </c>
@@ -3056,7 +3061,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>210</v>
       </c>
@@ -3067,7 +3072,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>213</v>
       </c>
@@ -3078,7 +3083,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>216</v>
       </c>
@@ -3089,7 +3094,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>219</v>
       </c>
@@ -3100,7 +3105,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>222</v>
       </c>
@@ -3111,7 +3116,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>225</v>
       </c>
@@ -3122,7 +3127,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>228</v>
       </c>
@@ -3133,7 +3138,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>231</v>
       </c>
@@ -3144,7 +3149,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>234</v>
       </c>
@@ -3155,7 +3160,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>237</v>
       </c>
@@ -3166,7 +3171,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>240</v>
       </c>
@@ -3177,7 +3182,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>243</v>
       </c>
@@ -3188,7 +3193,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>246</v>
       </c>
@@ -3199,7 +3204,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>249</v>
       </c>
@@ -3210,7 +3215,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>252</v>
       </c>
@@ -3221,7 +3226,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>255</v>
       </c>
@@ -3232,7 +3237,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>258</v>
       </c>
@@ -3243,7 +3248,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>260</v>
       </c>
@@ -3254,7 +3259,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>263</v>
       </c>
@@ -3265,7 +3270,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>266</v>
       </c>
@@ -3276,7 +3281,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>269</v>
       </c>
@@ -3287,7 +3292,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>272</v>
       </c>
@@ -3298,7 +3303,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>275</v>
       </c>
@@ -3309,7 +3314,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>278</v>
       </c>
@@ -3320,7 +3325,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>686</v>
       </c>
@@ -3331,7 +3336,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>281</v>
       </c>
@@ -3342,7 +3347,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>284</v>
       </c>
@@ -3353,7 +3358,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>287</v>
       </c>
@@ -3364,7 +3369,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>288</v>
       </c>
@@ -3375,7 +3380,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>291</v>
       </c>
@@ -3386,7 +3391,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>294</v>
       </c>
@@ -3397,7 +3402,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>297</v>
       </c>
@@ -3408,7 +3413,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>300</v>
       </c>
@@ -3419,7 +3424,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>303</v>
       </c>
@@ -3430,7 +3435,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>304</v>
       </c>
@@ -3441,7 +3446,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>307</v>
       </c>
@@ -3452,7 +3457,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>310</v>
       </c>
@@ -3463,7 +3468,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>313</v>
       </c>
@@ -3474,7 +3479,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>316</v>
       </c>
@@ -3485,7 +3490,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>319</v>
       </c>
@@ -3496,7 +3501,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>322</v>
       </c>
@@ -3507,7 +3512,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>325</v>
       </c>
@@ -3518,7 +3523,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>328</v>
       </c>
@@ -3529,7 +3534,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>331</v>
       </c>
@@ -3540,7 +3545,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>334</v>
       </c>
@@ -3551,7 +3556,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>337</v>
       </c>
@@ -3562,7 +3567,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>340</v>
       </c>
@@ -3573,7 +3578,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>343</v>
       </c>
@@ -3584,7 +3589,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>346</v>
       </c>
@@ -3595,7 +3600,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>349</v>
       </c>
@@ -3606,7 +3611,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>352</v>
       </c>
@@ -3617,7 +3622,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>355</v>
       </c>
@@ -3628,7 +3633,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>357</v>
       </c>
@@ -3639,7 +3644,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>358</v>
       </c>
@@ -3650,7 +3655,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>361</v>
       </c>
@@ -3661,7 +3666,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>362</v>
       </c>
@@ -3672,7 +3677,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>365</v>
       </c>
@@ -3683,7 +3688,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>366</v>
       </c>
@@ -3694,7 +3699,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>369</v>
       </c>
@@ -3705,7 +3710,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>372</v>
       </c>
@@ -3716,7 +3721,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>373</v>
       </c>
@@ -3727,7 +3732,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>376</v>
       </c>
@@ -3738,7 +3743,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>379</v>
       </c>
@@ -3749,7 +3754,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>382</v>
       </c>
@@ -3760,7 +3765,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>385</v>
       </c>
@@ -3771,7 +3776,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>388</v>
       </c>
@@ -3782,7 +3787,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>391</v>
       </c>
@@ -3793,7 +3798,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>394</v>
       </c>
@@ -3804,7 +3809,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>397</v>
       </c>
@@ -3815,7 +3820,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>400</v>
       </c>
@@ -3826,7 +3831,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>403</v>
       </c>
@@ -3837,7 +3842,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>406</v>
       </c>
@@ -3848,7 +3853,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>409</v>
       </c>
@@ -3859,7 +3864,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>412</v>
       </c>
@@ -3870,7 +3875,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>415</v>
       </c>
@@ -3881,7 +3886,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>418</v>
       </c>
@@ -3892,7 +3897,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>421</v>
       </c>
@@ -3903,7 +3908,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>424</v>
       </c>
@@ -3914,7 +3919,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>427</v>
       </c>
@@ -3925,7 +3930,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>430</v>
       </c>
@@ -3936,7 +3941,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>433</v>
       </c>
@@ -3947,7 +3952,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>436</v>
       </c>
@@ -3958,7 +3963,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>439</v>
       </c>
@@ -3969,7 +3974,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>442</v>
       </c>
@@ -3980,7 +3985,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>445</v>
       </c>
@@ -3991,7 +3996,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>448</v>
       </c>
@@ -4002,7 +4007,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>451</v>
       </c>
@@ -4013,7 +4018,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>454</v>
       </c>
@@ -4024,7 +4029,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>455</v>
       </c>
@@ -4035,7 +4040,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>458</v>
       </c>
@@ -4046,7 +4051,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>461</v>
       </c>
@@ -4057,7 +4062,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>464</v>
       </c>
@@ -4068,7 +4073,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>467</v>
       </c>
@@ -4079,7 +4084,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>470</v>
       </c>
@@ -4090,7 +4095,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>473</v>
       </c>
@@ -4101,7 +4106,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>474</v>
       </c>
@@ -4112,7 +4117,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>477</v>
       </c>
@@ -4123,7 +4128,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>480</v>
       </c>
@@ -4134,7 +4139,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>483</v>
       </c>
@@ -4145,7 +4150,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>486</v>
       </c>
@@ -4156,7 +4161,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>489</v>
       </c>
@@ -4167,7 +4172,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>492</v>
       </c>
@@ -4178,7 +4183,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>495</v>
       </c>
@@ -4189,7 +4194,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>498</v>
       </c>
@@ -4200,7 +4205,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>499</v>
       </c>
@@ -4211,7 +4216,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>502</v>
       </c>
@@ -4222,7 +4227,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>505</v>
       </c>
@@ -4233,7 +4238,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>508</v>
       </c>
@@ -4244,7 +4249,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>690</v>
       </c>
@@ -4255,7 +4260,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>509</v>
       </c>
@@ -4266,7 +4271,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>510</v>
       </c>
@@ -4277,7 +4282,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>511</v>
       </c>
@@ -4288,7 +4293,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>514</v>
       </c>
@@ -4299,7 +4304,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>515</v>
       </c>
@@ -4310,7 +4315,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>518</v>
       </c>
@@ -4321,7 +4326,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>682</v>
       </c>
@@ -4332,7 +4337,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>683</v>
       </c>
@@ -4343,7 +4348,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>519</v>
       </c>
@@ -4354,7 +4359,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>522</v>
       </c>
@@ -4365,7 +4370,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>525</v>
       </c>
@@ -4376,7 +4381,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>526</v>
       </c>
@@ -4387,7 +4392,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>527</v>
       </c>
@@ -4398,7 +4403,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>528</v>
       </c>
@@ -4409,7 +4414,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>529</v>
       </c>
@@ -4420,7 +4425,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>532</v>
       </c>
@@ -4431,7 +4436,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>535</v>
       </c>
@@ -4442,7 +4447,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>538</v>
       </c>
@@ -4453,7 +4458,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>541</v>
       </c>
@@ -4464,7 +4469,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>544</v>
       </c>
@@ -4475,7 +4480,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>547</v>
       </c>
@@ -4486,7 +4491,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>550</v>
       </c>
@@ -4497,7 +4502,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>553</v>
       </c>
@@ -4508,7 +4513,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>556</v>
       </c>
@@ -4519,7 +4524,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>557</v>
       </c>
@@ -4530,7 +4535,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>560</v>
       </c>
@@ -4541,7 +4546,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>563</v>
       </c>
@@ -4552,7 +4557,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>566</v>
       </c>
@@ -4563,7 +4568,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>569</v>
       </c>
@@ -4574,7 +4579,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>572</v>
       </c>
@@ -4585,7 +4590,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>575</v>
       </c>
@@ -4596,7 +4601,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>576</v>
       </c>
@@ -4607,7 +4612,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>579</v>
       </c>
@@ -4618,7 +4623,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>582</v>
       </c>
@@ -4629,7 +4634,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>585</v>
       </c>
@@ -4640,7 +4645,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>586</v>
       </c>
@@ -4651,7 +4656,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>589</v>
       </c>
@@ -4662,7 +4667,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>592</v>
       </c>
@@ -4673,7 +4678,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>593</v>
       </c>
@@ -4684,7 +4689,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>594</v>
       </c>
@@ -4695,7 +4700,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>597</v>
       </c>
@@ -4706,7 +4711,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>600</v>
       </c>
@@ -4717,7 +4722,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>603</v>
       </c>
@@ -4728,7 +4733,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>606</v>
       </c>
@@ -4739,7 +4744,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>609</v>
       </c>
@@ -4750,7 +4755,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>612</v>
       </c>
@@ -4761,7 +4766,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>615</v>
       </c>
@@ -4772,7 +4777,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>618</v>
       </c>
@@ -4783,7 +4788,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>621</v>
       </c>
@@ -4794,7 +4799,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>624</v>
       </c>
@@ -4805,7 +4810,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>627</v>
       </c>
@@ -4816,7 +4821,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>630</v>
       </c>
@@ -4827,7 +4832,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>633</v>
       </c>
@@ -4838,7 +4843,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>636</v>
       </c>
@@ -4849,7 +4854,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>639</v>
       </c>
@@ -4860,7 +4865,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>642</v>
       </c>
@@ -4871,7 +4876,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>645</v>
       </c>
@@ -4882,7 +4887,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>648</v>
       </c>
@@ -4893,7 +4898,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>651</v>
       </c>
@@ -4904,7 +4909,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>654</v>
       </c>
@@ -4915,7 +4920,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>657</v>
       </c>
@@ -4926,7 +4931,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>660</v>
       </c>
@@ -4937,7 +4942,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>663</v>
       </c>
@@ -4948,7 +4953,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>666</v>
       </c>
@@ -4959,7 +4964,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>669</v>
       </c>
@@ -4970,7 +4975,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>670</v>
       </c>
@@ -4981,7 +4986,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>671</v>
       </c>
@@ -4992,7 +4997,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>674</v>
       </c>
@@ -5003,7 +5008,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>677</v>
       </c>
@@ -5014,7 +5019,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>679</v>
       </c>
@@ -5025,7 +5030,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>0</v>
       </c>
@@ -5036,7 +5041,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>3</v>
       </c>
@@ -5047,7 +5052,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>6</v>
       </c>
@@ -5058,7 +5063,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>9</v>
       </c>
@@ -5069,7 +5074,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>12</v>
       </c>
@@ -5080,7 +5085,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>15</v>
       </c>
@@ -5091,7 +5096,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>18</v>
       </c>
@@ -5102,7 +5107,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>21</v>
       </c>
@@ -5113,7 +5118,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>24</v>
       </c>
@@ -5124,7 +5129,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>27</v>
       </c>
@@ -5135,7 +5140,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>30</v>
       </c>
@@ -5146,7 +5151,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>33</v>
       </c>
@@ -5157,7 +5162,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>36</v>
       </c>
@@ -5168,7 +5173,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>37</v>
       </c>
@@ -5179,7 +5184,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>38</v>
       </c>
@@ -5190,7 +5195,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>41</v>
       </c>
@@ -5201,7 +5206,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>44</v>
       </c>
@@ -5212,7 +5217,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>47</v>
       </c>
@@ -5223,7 +5228,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>50</v>
       </c>
@@ -5234,7 +5239,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>53</v>
       </c>
@@ -5245,7 +5250,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>56</v>
       </c>
@@ -5256,7 +5261,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>59</v>
       </c>
@@ -5267,7 +5272,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>62</v>
       </c>
@@ -5278,7 +5283,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>65</v>
       </c>
@@ -5289,7 +5294,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>687</v>
       </c>
@@ -5298,6 +5303,17 @@
       </c>
       <c r="C257" t="s">
         <v>689</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="B258" t="s">
+        <v>646</v>
+      </c>
+      <c r="C258" t="s">
+        <v>647</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
varios csv the HC y NHC updats en sp_index
</commit_message>
<xml_diff>
--- a/clean_databases/sp_index.xlsx
+++ b/clean_databases/sp_index.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27510"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignacia Rivera\Desktop\GitHub\main-fisheries-chile\clean_databases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargaspoulsen/github/main-fisheries-chile/clean_databases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20779364-35ED-4F2B-8B92-706DD416CC16}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25455" windowHeight="15465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25460" windowHeight="15460"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,18 +19,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="693">
   <si>
     <t>HAEMATOCOCCUS</t>
   </si>
@@ -2107,12 +2106,15 @@
   </si>
   <si>
     <t>ATUN LISTADO,BARRILETE,CACHURRETA/AUHOPU</t>
+  </si>
+  <si>
+    <t>NANUE, NANUE PARA, PISI O PUA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2464,21 +2466,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C258"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
-      <selection activeCell="D254" sqref="D254"/>
+    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
+      <selection activeCell="B232" sqref="B232:C232"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -2489,7 +2491,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -2500,7 +2502,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -2511,7 +2513,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -2522,7 +2524,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -2533,7 +2535,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>83</v>
       </c>
@@ -2544,7 +2546,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>86</v>
       </c>
@@ -2555,7 +2557,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>89</v>
       </c>
@@ -2566,7 +2568,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>92</v>
       </c>
@@ -2577,7 +2579,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -2588,7 +2590,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>98</v>
       </c>
@@ -2599,7 +2601,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -2610,7 +2612,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>104</v>
       </c>
@@ -2621,7 +2623,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>107</v>
       </c>
@@ -2632,7 +2634,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>110</v>
       </c>
@@ -2643,7 +2645,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>111</v>
       </c>
@@ -2654,7 +2656,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>114</v>
       </c>
@@ -2665,7 +2667,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>117</v>
       </c>
@@ -2676,7 +2678,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>119</v>
       </c>
@@ -2687,7 +2689,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>122</v>
       </c>
@@ -2698,7 +2700,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>125</v>
       </c>
@@ -2709,7 +2711,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -2720,7 +2722,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>129</v>
       </c>
@@ -2731,7 +2733,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>130</v>
       </c>
@@ -2742,7 +2744,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>131</v>
       </c>
@@ -2753,7 +2755,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>132</v>
       </c>
@@ -2764,7 +2766,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>135</v>
       </c>
@@ -2775,7 +2777,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>138</v>
       </c>
@@ -2786,7 +2788,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -2797,7 +2799,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>144</v>
       </c>
@@ -2808,7 +2810,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>145</v>
       </c>
@@ -2819,7 +2821,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>148</v>
       </c>
@@ -2830,7 +2832,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>151</v>
       </c>
@@ -2841,7 +2843,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>154</v>
       </c>
@@ -2852,7 +2854,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>685</v>
       </c>
@@ -2863,7 +2865,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>156</v>
       </c>
@@ -2874,7 +2876,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>159</v>
       </c>
@@ -2885,7 +2887,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>162</v>
       </c>
@@ -2896,7 +2898,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>165</v>
       </c>
@@ -2907,7 +2909,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>168</v>
       </c>
@@ -2918,7 +2920,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>171</v>
       </c>
@@ -2929,7 +2931,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>174</v>
       </c>
@@ -2940,7 +2942,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>177</v>
       </c>
@@ -2951,7 +2953,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>180</v>
       </c>
@@ -2962,7 +2964,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>183</v>
       </c>
@@ -2973,7 +2975,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>186</v>
       </c>
@@ -2984,7 +2986,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>189</v>
       </c>
@@ -2995,7 +2997,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>192</v>
       </c>
@@ -3006,7 +3008,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>195</v>
       </c>
@@ -3017,7 +3019,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>198</v>
       </c>
@@ -3028,7 +3030,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>201</v>
       </c>
@@ -3039,7 +3041,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>204</v>
       </c>
@@ -3050,7 +3052,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>207</v>
       </c>
@@ -3061,7 +3063,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>210</v>
       </c>
@@ -3072,7 +3074,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>213</v>
       </c>
@@ -3083,7 +3085,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>216</v>
       </c>
@@ -3094,7 +3096,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>219</v>
       </c>
@@ -3105,7 +3107,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>222</v>
       </c>
@@ -3116,7 +3118,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>225</v>
       </c>
@@ -3127,7 +3129,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>228</v>
       </c>
@@ -3138,7 +3140,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>231</v>
       </c>
@@ -3149,7 +3151,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>234</v>
       </c>
@@ -3160,7 +3162,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>237</v>
       </c>
@@ -3171,7 +3173,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>240</v>
       </c>
@@ -3182,7 +3184,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>243</v>
       </c>
@@ -3193,7 +3195,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>246</v>
       </c>
@@ -3204,7 +3206,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>249</v>
       </c>
@@ -3215,7 +3217,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>252</v>
       </c>
@@ -3226,7 +3228,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>255</v>
       </c>
@@ -3237,7 +3239,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>258</v>
       </c>
@@ -3248,7 +3250,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>260</v>
       </c>
@@ -3259,7 +3261,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>263</v>
       </c>
@@ -3270,7 +3272,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>266</v>
       </c>
@@ -3281,7 +3283,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>269</v>
       </c>
@@ -3292,7 +3294,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>272</v>
       </c>
@@ -3303,7 +3305,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>275</v>
       </c>
@@ -3314,7 +3316,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>278</v>
       </c>
@@ -3325,7 +3327,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>686</v>
       </c>
@@ -3336,7 +3338,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>281</v>
       </c>
@@ -3347,7 +3349,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>284</v>
       </c>
@@ -3358,7 +3360,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>287</v>
       </c>
@@ -3369,7 +3371,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>288</v>
       </c>
@@ -3380,7 +3382,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>291</v>
       </c>
@@ -3391,7 +3393,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>294</v>
       </c>
@@ -3402,7 +3404,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>297</v>
       </c>
@@ -3413,7 +3415,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>300</v>
       </c>
@@ -3424,7 +3426,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>303</v>
       </c>
@@ -3435,7 +3437,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>304</v>
       </c>
@@ -3446,7 +3448,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>307</v>
       </c>
@@ -3457,7 +3459,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>310</v>
       </c>
@@ -3468,7 +3470,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>313</v>
       </c>
@@ -3479,7 +3481,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>316</v>
       </c>
@@ -3490,7 +3492,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>319</v>
       </c>
@@ -3501,7 +3503,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>322</v>
       </c>
@@ -3512,7 +3514,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>325</v>
       </c>
@@ -3523,7 +3525,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>328</v>
       </c>
@@ -3534,7 +3536,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>331</v>
       </c>
@@ -3545,7 +3547,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>334</v>
       </c>
@@ -3556,7 +3558,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>337</v>
       </c>
@@ -3567,7 +3569,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>340</v>
       </c>
@@ -3578,7 +3580,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>343</v>
       </c>
@@ -3589,7 +3591,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>346</v>
       </c>
@@ -3600,7 +3602,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>349</v>
       </c>
@@ -3611,7 +3613,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>352</v>
       </c>
@@ -3622,7 +3624,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>355</v>
       </c>
@@ -3633,7 +3635,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>357</v>
       </c>
@@ -3644,7 +3646,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>358</v>
       </c>
@@ -3655,7 +3657,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>361</v>
       </c>
@@ -3666,7 +3668,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>362</v>
       </c>
@@ -3677,7 +3679,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>365</v>
       </c>
@@ -3688,7 +3690,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>366</v>
       </c>
@@ -3699,7 +3701,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>369</v>
       </c>
@@ -3710,7 +3712,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>372</v>
       </c>
@@ -3721,7 +3723,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>373</v>
       </c>
@@ -3732,7 +3734,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>376</v>
       </c>
@@ -3743,7 +3745,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>379</v>
       </c>
@@ -3754,7 +3756,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>382</v>
       </c>
@@ -3765,7 +3767,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>385</v>
       </c>
@@ -3776,7 +3778,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>388</v>
       </c>
@@ -3787,7 +3789,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>391</v>
       </c>
@@ -3798,7 +3800,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>394</v>
       </c>
@@ -3809,7 +3811,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>397</v>
       </c>
@@ -3820,7 +3822,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>400</v>
       </c>
@@ -3831,7 +3833,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>403</v>
       </c>
@@ -3842,7 +3844,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>406</v>
       </c>
@@ -3853,7 +3855,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>409</v>
       </c>
@@ -3864,7 +3866,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>412</v>
       </c>
@@ -3875,7 +3877,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>415</v>
       </c>
@@ -3886,7 +3888,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>418</v>
       </c>
@@ -3897,7 +3899,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>421</v>
       </c>
@@ -3908,7 +3910,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>424</v>
       </c>
@@ -3919,7 +3921,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>427</v>
       </c>
@@ -3930,7 +3932,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>430</v>
       </c>
@@ -3941,7 +3943,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>433</v>
       </c>
@@ -3952,7 +3954,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>436</v>
       </c>
@@ -3963,7 +3965,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>439</v>
       </c>
@@ -3974,7 +3976,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>442</v>
       </c>
@@ -3985,7 +3987,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>445</v>
       </c>
@@ -3996,7 +3998,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>448</v>
       </c>
@@ -4007,7 +4009,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>451</v>
       </c>
@@ -4018,7 +4020,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>454</v>
       </c>
@@ -4029,7 +4031,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>455</v>
       </c>
@@ -4040,7 +4042,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>458</v>
       </c>
@@ -4051,7 +4053,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>461</v>
       </c>
@@ -4062,7 +4064,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>464</v>
       </c>
@@ -4073,7 +4075,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>467</v>
       </c>
@@ -4084,7 +4086,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>470</v>
       </c>
@@ -4095,7 +4097,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>473</v>
       </c>
@@ -4106,7 +4108,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>474</v>
       </c>
@@ -4117,7 +4119,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>477</v>
       </c>
@@ -4128,7 +4130,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>480</v>
       </c>
@@ -4139,7 +4141,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>483</v>
       </c>
@@ -4150,7 +4152,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>486</v>
       </c>
@@ -4161,7 +4163,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>489</v>
       </c>
@@ -4172,7 +4174,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>492</v>
       </c>
@@ -4183,7 +4185,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>495</v>
       </c>
@@ -4194,7 +4196,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>498</v>
       </c>
@@ -4205,7 +4207,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>499</v>
       </c>
@@ -4216,7 +4218,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>502</v>
       </c>
@@ -4227,7 +4229,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>505</v>
       </c>
@@ -4238,7 +4240,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>508</v>
       </c>
@@ -4249,7 +4251,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>690</v>
       </c>
@@ -4260,7 +4262,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>509</v>
       </c>
@@ -4271,7 +4273,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>510</v>
       </c>
@@ -4282,7 +4284,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>511</v>
       </c>
@@ -4293,7 +4295,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>514</v>
       </c>
@@ -4304,7 +4306,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>515</v>
       </c>
@@ -4315,7 +4317,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>518</v>
       </c>
@@ -4326,7 +4328,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>682</v>
       </c>
@@ -4337,7 +4339,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>683</v>
       </c>
@@ -4348,7 +4350,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>519</v>
       </c>
@@ -4359,7 +4361,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>522</v>
       </c>
@@ -4370,7 +4372,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>525</v>
       </c>
@@ -4381,7 +4383,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>526</v>
       </c>
@@ -4392,7 +4394,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>527</v>
       </c>
@@ -4403,7 +4405,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>528</v>
       </c>
@@ -4414,7 +4416,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>529</v>
       </c>
@@ -4425,7 +4427,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>532</v>
       </c>
@@ -4436,7 +4438,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>535</v>
       </c>
@@ -4447,7 +4449,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>538</v>
       </c>
@@ -4458,7 +4460,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>541</v>
       </c>
@@ -4469,7 +4471,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>544</v>
       </c>
@@ -4480,7 +4482,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>547</v>
       </c>
@@ -4491,7 +4493,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>550</v>
       </c>
@@ -4502,7 +4504,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>553</v>
       </c>
@@ -4513,7 +4515,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>556</v>
       </c>
@@ -4524,7 +4526,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>557</v>
       </c>
@@ -4535,7 +4537,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>560</v>
       </c>
@@ -4546,7 +4548,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>563</v>
       </c>
@@ -4557,7 +4559,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>566</v>
       </c>
@@ -4568,7 +4570,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>569</v>
       </c>
@@ -4579,7 +4581,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>572</v>
       </c>
@@ -4590,7 +4592,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>575</v>
       </c>
@@ -4601,7 +4603,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>576</v>
       </c>
@@ -4612,7 +4614,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>579</v>
       </c>
@@ -4623,7 +4625,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>582</v>
       </c>
@@ -4634,7 +4636,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>585</v>
       </c>
@@ -4645,7 +4647,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>586</v>
       </c>
@@ -4656,7 +4658,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>589</v>
       </c>
@@ -4667,7 +4669,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>592</v>
       </c>
@@ -4678,7 +4680,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>593</v>
       </c>
@@ -4689,7 +4691,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>594</v>
       </c>
@@ -4700,7 +4702,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>597</v>
       </c>
@@ -4711,7 +4713,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>600</v>
       </c>
@@ -4722,7 +4724,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>603</v>
       </c>
@@ -4733,7 +4735,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>606</v>
       </c>
@@ -4744,7 +4746,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>609</v>
       </c>
@@ -4755,7 +4757,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>612</v>
       </c>
@@ -4766,7 +4768,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>615</v>
       </c>
@@ -4777,7 +4779,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>618</v>
       </c>
@@ -4788,7 +4790,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>621</v>
       </c>
@@ -4799,7 +4801,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>624</v>
       </c>
@@ -4810,7 +4812,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>627</v>
       </c>
@@ -4821,7 +4823,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>630</v>
       </c>
@@ -4832,7 +4834,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>633</v>
       </c>
@@ -4843,7 +4845,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>636</v>
       </c>
@@ -4854,7 +4856,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>639</v>
       </c>
@@ -4865,7 +4867,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>642</v>
       </c>
@@ -4876,7 +4878,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>645</v>
       </c>
@@ -4887,7 +4889,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>648</v>
       </c>
@@ -4898,7 +4900,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>651</v>
       </c>
@@ -4909,7 +4911,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>654</v>
       </c>
@@ -4920,7 +4922,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>657</v>
       </c>
@@ -4931,7 +4933,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>660</v>
       </c>
@@ -4942,7 +4944,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>663</v>
       </c>
@@ -4953,7 +4955,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>666</v>
       </c>
@@ -4964,7 +4966,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>669</v>
       </c>
@@ -4975,7 +4977,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>670</v>
       </c>
@@ -4986,7 +4988,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>671</v>
       </c>
@@ -4997,7 +4999,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>674</v>
       </c>
@@ -5008,7 +5010,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>677</v>
       </c>
@@ -5019,300 +5021,311 @@
         <v>390</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
+        <v>692</v>
+      </c>
+      <c r="B232" t="s">
+        <v>678</v>
+      </c>
+      <c r="C232" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
         <v>679</v>
       </c>
-      <c r="B232" t="s">
+      <c r="B233" t="s">
         <v>680</v>
       </c>
-      <c r="C232" t="s">
+      <c r="C233" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
         <v>0</v>
       </c>
-      <c r="B233" t="s">
+      <c r="B234" t="s">
         <v>1</v>
       </c>
-      <c r="C233" t="s">
+      <c r="C234" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A234" t="s">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
         <v>3</v>
       </c>
-      <c r="B234" t="s">
+      <c r="B235" t="s">
         <v>4</v>
       </c>
-      <c r="C234" t="s">
+      <c r="C235" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A235" t="s">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
         <v>6</v>
       </c>
-      <c r="B235" t="s">
+      <c r="B236" t="s">
         <v>7</v>
       </c>
-      <c r="C235" t="s">
+      <c r="C236" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A236" t="s">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
         <v>9</v>
       </c>
-      <c r="B236" t="s">
+      <c r="B237" t="s">
         <v>10</v>
       </c>
-      <c r="C236" t="s">
+      <c r="C237" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A237" t="s">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
         <v>12</v>
       </c>
-      <c r="B237" t="s">
+      <c r="B238" t="s">
         <v>13</v>
       </c>
-      <c r="C237" t="s">
+      <c r="C238" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
         <v>15</v>
       </c>
-      <c r="B238" t="s">
+      <c r="B239" t="s">
         <v>16</v>
       </c>
-      <c r="C238" t="s">
+      <c r="C239" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A239" t="s">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
         <v>18</v>
       </c>
-      <c r="B239" t="s">
+      <c r="B240" t="s">
         <v>19</v>
       </c>
-      <c r="C239" t="s">
+      <c r="C240" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A240" t="s">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
         <v>21</v>
       </c>
-      <c r="B240" t="s">
+      <c r="B241" t="s">
         <v>22</v>
       </c>
-      <c r="C240" t="s">
+      <c r="C241" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A241" t="s">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
         <v>24</v>
       </c>
-      <c r="B241" t="s">
+      <c r="B242" t="s">
         <v>25</v>
       </c>
-      <c r="C241" t="s">
+      <c r="C242" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A242" t="s">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
         <v>27</v>
       </c>
-      <c r="B242" t="s">
+      <c r="B243" t="s">
         <v>28</v>
       </c>
-      <c r="C242" t="s">
+      <c r="C243" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A243" t="s">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
         <v>30</v>
       </c>
-      <c r="B243" t="s">
+      <c r="B244" t="s">
         <v>31</v>
       </c>
-      <c r="C243" t="s">
+      <c r="C244" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A244" t="s">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
         <v>33</v>
       </c>
-      <c r="B244" t="s">
+      <c r="B245" t="s">
         <v>34</v>
       </c>
-      <c r="C244" t="s">
+      <c r="C245" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A245" t="s">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
         <v>36</v>
       </c>
-      <c r="B245" t="s">
+      <c r="B246" t="s">
         <v>16</v>
       </c>
-      <c r="C245" t="s">
+      <c r="C246" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A246" t="s">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
         <v>37</v>
       </c>
-      <c r="B246" t="s">
+      <c r="B247" t="s">
         <v>19</v>
       </c>
-      <c r="C246" t="s">
+      <c r="C247" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A247" t="s">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
         <v>38</v>
       </c>
-      <c r="B247" t="s">
+      <c r="B248" t="s">
         <v>39</v>
       </c>
-      <c r="C247" t="s">
+      <c r="C248" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A248" t="s">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
         <v>41</v>
       </c>
-      <c r="B248" t="s">
+      <c r="B249" t="s">
         <v>42</v>
       </c>
-      <c r="C248" t="s">
+      <c r="C249" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A249" t="s">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
         <v>44</v>
       </c>
-      <c r="B249" t="s">
+      <c r="B250" t="s">
         <v>45</v>
       </c>
-      <c r="C249" t="s">
+      <c r="C250" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A250" t="s">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
         <v>47</v>
       </c>
-      <c r="B250" t="s">
+      <c r="B251" t="s">
         <v>48</v>
       </c>
-      <c r="C250" t="s">
+      <c r="C251" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A251" t="s">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
         <v>50</v>
       </c>
-      <c r="B251" t="s">
+      <c r="B252" t="s">
         <v>51</v>
       </c>
-      <c r="C251" t="s">
+      <c r="C252" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A252" t="s">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
         <v>53</v>
       </c>
-      <c r="B252" t="s">
+      <c r="B253" t="s">
         <v>54</v>
       </c>
-      <c r="C252" t="s">
+      <c r="C253" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A253" t="s">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
         <v>56</v>
       </c>
-      <c r="B253" t="s">
+      <c r="B254" t="s">
         <v>57</v>
       </c>
-      <c r="C253" t="s">
+      <c r="C254" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A254" t="s">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
         <v>59</v>
       </c>
-      <c r="B254" t="s">
+      <c r="B255" t="s">
         <v>60</v>
       </c>
-      <c r="C254" t="s">
+      <c r="C255" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A255" t="s">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
         <v>62</v>
       </c>
-      <c r="B255" t="s">
+      <c r="B256" t="s">
         <v>63</v>
       </c>
-      <c r="C255" t="s">
+      <c r="C256" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A256" t="s">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A257" t="s">
         <v>65</v>
       </c>
-      <c r="B256" t="s">
+      <c r="B257" t="s">
         <v>66</v>
       </c>
-      <c r="C256" t="s">
+      <c r="C257" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A257" t="s">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A258" t="s">
         <v>687</v>
       </c>
-      <c r="B257" t="s">
+      <c r="B258" t="s">
         <v>688</v>
       </c>
-      <c r="C257" t="s">
+      <c r="C258" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A258" s="1" t="s">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A259" s="1" t="s">
         <v>691</v>
       </c>
-      <c r="B258" t="s">
+      <c r="B259" t="s">
         <v>646</v>
       </c>
-      <c r="C258" t="s">
+      <c r="C259" t="s">
         <v>647</v>
       </c>
     </row>

</xml_diff>